<commit_message>
Update on 3/11/2025 at 9:26pm
</commit_message>
<xml_diff>
--- a/mmc_enrollment_vs_spending.xlsx
+++ b/mmc_enrollment_vs_spending.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac/Documents/RProjects/s2p_data_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D79843-3777-9548-9CB5-958D16CCC3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFC7074-F341-7643-8930-0A0004056F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1098,7 +1098,6 @@
     <xf numFmtId="166" fontId="8" fillId="3" borderId="4" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="8" fillId="3" borderId="21" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1135,6 +1134,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent4" xfId="11" builtinId="42"/>
@@ -3596,7 +3598,7 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3607,42 +3609,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:13" s="15" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48" t="s">
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50" t="s">
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="1:13" s="26" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
@@ -4634,7 +4636,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4655,20 +4657,20 @@
   <sheetData>
     <row r="1" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P2" s="61" t="s">
+      <c r="P2" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="63"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="62"/>
     </row>
     <row r="3" spans="16:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="P3" s="64" t="s">
+      <c r="P3" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="66"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="65"/>
     </row>
     <row r="4" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P4" s="19"/>
@@ -4677,12 +4679,12 @@
       <c r="S4" s="21"/>
     </row>
     <row r="5" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="58" t="s">
+      <c r="P5" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="60"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="59"/>
     </row>
     <row r="6" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P6" s="10" t="s">
@@ -4724,12 +4726,12 @@
       <c r="S9" s="21"/>
     </row>
     <row r="10" spans="16:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P10" s="58" t="s">
+      <c r="P10" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="60"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="59"/>
     </row>
     <row r="11" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P11" s="10" t="s">
@@ -4771,12 +4773,12 @@
       <c r="S14" s="21"/>
     </row>
     <row r="15" spans="16:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="55" t="s">
+      <c r="P15" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="57"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="56"/>
     </row>
     <row r="16" spans="16:19" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="P16" s="37" t="s">
@@ -4787,18 +4789,18 @@
       <c r="S16" s="21"/>
     </row>
     <row r="17" spans="16:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P17" s="52" t="s">
+      <c r="P17" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="54"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="53"/>
     </row>
     <row r="18" spans="16:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P18" s="52"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="54"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="53"/>
     </row>
     <row r="19" spans="16:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P19" s="22" t="s">
@@ -4814,7 +4816,7 @@
         <v>4.36E-2</v>
       </c>
       <c r="Q20" s="7"/>
-      <c r="R20" s="46">
+      <c r="R20" s="66">
         <v>2.4E-2</v>
       </c>
       <c r="S20" s="9"/>

</xml_diff>